<commit_message>
optical sensor AliExpress Vendor Removed
</commit_message>
<xml_diff>
--- a/bom/BOM_BMGAqua.xlsx
+++ b/bom/BOM_BMGAqua.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8bf86f88c49aa82/Documents/GitHub/HevORT/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{2DD0808E-D91E-4CEE-8509-F948C81AB46F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4D814616-FD7E-4EBF-A5A6-1AED6A3BF377}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="13_ncr:1_{2DD0808E-D91E-4CEE-8509-F948C81AB46F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{26A11555-BC8A-4AD5-891B-5332FFA69A40}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="98">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -296,12 +296,6 @@
   </si>
   <si>
     <t>Optical End-Stop</t>
-  </si>
-  <si>
-    <t>AliExpress</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/33006421501.html?spm=a2g0s.9042311.0.0.3e4d4c4dQtB9Y8</t>
   </si>
   <si>
     <t>37ae3e0660b16d0dba47ce09569758c1</t>
@@ -422,6 +416,15 @@
   </cellStyles>
   <dxfs count="14">
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -439,21 +442,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -491,6 +479,12 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1993,18 +1987,18 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD53AF23-1354-4F84-BC9A-82BCD84E6CF8}" name="Table1" displayName="Table1" ref="A1:L34" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:L34" xr:uid="{12DD6FC5-2D7E-4AEA-A165-7B8F7A73525C}"/>
   <tableColumns count="12">
-    <tableColumn id="11" xr3:uid="{592544CB-8C56-406F-B1D1-D85B040BBD7D}" name="SubAssy" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{63F8132C-2727-48B6-A5DF-EB9A9C6767FB}" name="Category" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{40B9773F-8FF2-45ED-BA4C-EA310F488575}" name="Thumbnail" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{B4FAF445-2DA8-4A6F-AA2A-4C4ECC9923AF}" name="Part Name" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{FB748403-76BD-425C-BF28-38F2516265B5}" name="Part Number" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{AEEF731D-14AE-4057-ABFF-ADF3E937D16C}" name="Description" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{BF89E185-62F4-4916-B520-18F71EEECBD3}" name="Make/Buy" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{B6F715AD-B7D8-4C11-B387-27E88FDA2F3A}" name="Quantity" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{A8451F80-DCC2-448F-B8D8-1508465A986D}" name="Comment" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{3BE6559A-C4DB-482F-AA15-35D31B25ECB0}" name="Vendor" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{466301A8-0BB1-4C3A-A6A4-EB6234BB3651}" name="Vendor URL" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{19062B6E-C67B-4605-92F6-F5F25F663C22}" name="Fusion360 ID" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{592544CB-8C56-406F-B1D1-D85B040BBD7D}" name="SubAssy" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{63F8132C-2727-48B6-A5DF-EB9A9C6767FB}" name="Category" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{40B9773F-8FF2-45ED-BA4C-EA310F488575}" name="Thumbnail" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{B4FAF445-2DA8-4A6F-AA2A-4C4ECC9923AF}" name="Part Name" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{FB748403-76BD-425C-BF28-38F2516265B5}" name="Part Number" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{AEEF731D-14AE-4057-ABFF-ADF3E937D16C}" name="Description" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{BF89E185-62F4-4916-B520-18F71EEECBD3}" name="Make/Buy" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{B6F715AD-B7D8-4C11-B387-27E88FDA2F3A}" name="Quantity" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{A8451F80-DCC2-448F-B8D8-1508465A986D}" name="Comment" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{3BE6559A-C4DB-482F-AA15-35D31B25ECB0}" name="Vendor" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{466301A8-0BB1-4C3A-A6A4-EB6234BB3651}" name="Vendor URL" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{19062B6E-C67B-4605-92F6-F5F25F663C22}" name="Fusion360 ID" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2333,8 +2327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
@@ -2354,10 +2348,10 @@
   <sheetData>
     <row r="1" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -2378,7 +2372,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
@@ -2387,15 +2381,15 @@
         <v>7</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>15</v>
@@ -2418,10 +2412,10 @@
     </row>
     <row r="3" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>19</v>
@@ -2444,10 +2438,10 @@
     </row>
     <row r="4" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>30</v>
@@ -2470,10 +2464,10 @@
     </row>
     <row r="5" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>33</v>
@@ -2496,10 +2490,10 @@
     </row>
     <row r="6" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>36</v>
@@ -2522,7 +2516,7 @@
     </row>
     <row r="7" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>17</v>
@@ -2545,7 +2539,7 @@
     </row>
     <row r="8" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>17</v>
@@ -2568,10 +2562,10 @@
     </row>
     <row r="9" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>43</v>
@@ -2594,10 +2588,10 @@
     </row>
     <row r="10" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>46</v>
@@ -2620,10 +2614,10 @@
     </row>
     <row r="11" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>49</v>
@@ -2646,10 +2640,10 @@
     </row>
     <row r="12" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>52</v>
@@ -2672,7 +2666,7 @@
     </row>
     <row r="13" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>17</v>
@@ -2695,7 +2689,7 @@
     </row>
     <row r="14" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>17</v>
@@ -2718,10 +2712,10 @@
     </row>
     <row r="15" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>61</v>
@@ -2744,10 +2738,10 @@
     </row>
     <row r="16" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>64</v>
@@ -2770,10 +2764,10 @@
     </row>
     <row r="17" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>67</v>
@@ -2796,10 +2790,10 @@
     </row>
     <row r="18" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>70</v>
@@ -2822,10 +2816,10 @@
     </row>
     <row r="19" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>73</v>
@@ -2848,7 +2842,7 @@
     </row>
     <row r="20" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>17</v>
@@ -2871,10 +2865,10 @@
     </row>
     <row r="21" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>86</v>
@@ -2897,7 +2891,7 @@
     </row>
     <row r="22" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>17</v>
@@ -2917,19 +2911,14 @@
       <c r="H22" s="6">
         <v>1</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="K22" s="3"/>
+      <c r="L22" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>9</v>
@@ -2952,7 +2941,7 @@
     </row>
     <row r="24" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>9</v>
@@ -2975,7 +2964,7 @@
     </row>
     <row r="25" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>9</v>
@@ -2998,7 +2987,7 @@
     </row>
     <row r="26" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>9</v>
@@ -3021,7 +3010,7 @@
     </row>
     <row r="27" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>9</v>
@@ -3044,7 +3033,7 @@
     </row>
     <row r="28" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>9</v>
@@ -3067,7 +3056,7 @@
     </row>
     <row r="29" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>9</v>
@@ -3090,7 +3079,7 @@
     </row>
     <row r="30" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>9</v>
@@ -3113,7 +3102,7 @@
     </row>
     <row r="31" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>9</v>
@@ -3136,7 +3125,7 @@
     </row>
     <row r="32" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>9</v>
@@ -3159,7 +3148,7 @@
     </row>
     <row r="33" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>9</v>
@@ -3182,7 +3171,7 @@
     </row>
     <row r="34" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>9</v>
@@ -3205,17 +3194,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="K22" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <webPublishItems count="1">
     <webPublishItem id="2101" divId="BOM_BMGAqua_2101" sourceType="sheet" destinationFile="https://d.docs.live.net/e8bf86f88c49aa82/Documents/GitHub/HevORT/bom/BOM_BMGAqua.htm" autoRepublish="1"/>
   </webPublishItems>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>